<commit_message>
Gerando hélice a partir da base
Beta e Corda não estão em relação linear?
Beta depende apenas de pitch e D
</commit_message>
<xml_diff>
--- a/2.MoyaLifterCruise1_57.0x37.9_B2_TMOTOR23kW_geom&performance-data_Rev01 (1) (1).xlsx
+++ b/2.MoyaLifterCruise1_57.0x37.9_B2_TMOTOR23kW_geom&performance-data_Rev01 (1) (1).xlsx
@@ -5,16 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://moyaaero.sharepoint.com/sites/MOYA-Engenharia-MOYA-760/Shared Documents/M-760/01 - 760/01 - Análises e Resultados/02 - Performance/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IC-TCC LPAA\TCC-GIT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F496E255-BF82-464F-ADE8-7B31E161F115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35EC6349-53B5-42E6-80CB-52DC908CB0C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1848" yWindow="1848" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{AB3C7112-BBE9-4033-AAE0-7D0F0EEB7533}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AB3C7112-BBE9-4033-AAE0-7D0F0EEB7533}"/>
   </bookViews>
   <sheets>
     <sheet name="Geometry" sheetId="2" r:id="rId1"/>
     <sheet name="Performance" sheetId="1" r:id="rId2"/>
+    <sheet name="Planilha1" sheetId="3" r:id="rId3"/>
+    <sheet name="Planilha2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -200,7 +202,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="100">
   <si>
     <t>V [m/s]</t>
   </si>
@@ -333,6 +335,174 @@
   <si>
     <t>P_nom</t>
   </si>
+  <si>
+    <t>0.1448</t>
+  </si>
+  <si>
+    <t>0.1186</t>
+  </si>
+  <si>
+    <t>0.181</t>
+  </si>
+  <si>
+    <t>0.1579</t>
+  </si>
+  <si>
+    <t>0.2172</t>
+  </si>
+  <si>
+    <t>0.1765</t>
+  </si>
+  <si>
+    <t>0.2534</t>
+  </si>
+  <si>
+    <t>0.1767</t>
+  </si>
+  <si>
+    <t>0.2896</t>
+  </si>
+  <si>
+    <t>0.1647</t>
+  </si>
+  <si>
+    <t>0.3258</t>
+  </si>
+  <si>
+    <t>0.1525</t>
+  </si>
+  <si>
+    <t>0.3619</t>
+  </si>
+  <si>
+    <t>0.1408</t>
+  </si>
+  <si>
+    <t>0.3981</t>
+  </si>
+  <si>
+    <t>0.1297</t>
+  </si>
+  <si>
+    <t>0.4343</t>
+  </si>
+  <si>
+    <t>0.1193</t>
+  </si>
+  <si>
+    <t>0.4705</t>
+  </si>
+  <si>
+    <t>0.1092</t>
+  </si>
+  <si>
+    <t>0.5067</t>
+  </si>
+  <si>
+    <t>0.0995</t>
+  </si>
+  <si>
+    <t>0.5429</t>
+  </si>
+  <si>
+    <t>0.0896</t>
+  </si>
+  <si>
+    <t>0.5791</t>
+  </si>
+  <si>
+    <t>0.0795</t>
+  </si>
+  <si>
+    <t>0.6153</t>
+  </si>
+  <si>
+    <t>0.0684</t>
+  </si>
+  <si>
+    <t>0.6515</t>
+  </si>
+  <si>
+    <t>0.0557</t>
+  </si>
+  <si>
+    <t>0.6877</t>
+  </si>
+  <si>
+    <t>0.0393</t>
+  </si>
+  <si>
+    <t>0.7058</t>
+  </si>
+  <si>
+    <t>0.0278</t>
+  </si>
+  <si>
+    <t>0.7167</t>
+  </si>
+  <si>
+    <t>0.0176</t>
+  </si>
+  <si>
+    <t>44.3</t>
+  </si>
+  <si>
+    <t>38.0</t>
+  </si>
+  <si>
+    <t>33.2</t>
+  </si>
+  <si>
+    <t>29.5</t>
+  </si>
+  <si>
+    <t>26.5</t>
+  </si>
+  <si>
+    <t>24.1</t>
+  </si>
+  <si>
+    <t>22.1</t>
+  </si>
+  <si>
+    <t>20.5</t>
+  </si>
+  <si>
+    <t>19.0</t>
+  </si>
+  <si>
+    <t>17.8</t>
+  </si>
+  <si>
+    <t>16.7</t>
+  </si>
+  <si>
+    <t>15.8</t>
+  </si>
+  <si>
+    <t>15.0</t>
+  </si>
+  <si>
+    <t>14.2</t>
+  </si>
+  <si>
+    <t>13.6</t>
+  </si>
+  <si>
+    <t>13.0</t>
+  </si>
+  <si>
+    <t>12.7</t>
+  </si>
+  <si>
+    <t>12.6</t>
+  </si>
+  <si>
+    <t>Pitch</t>
+  </si>
+  <si>
+    <t>B75 rad</t>
+  </si>
 </sst>
 </file>
 
@@ -419,7 +589,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -450,6 +620,13 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -555,6 +732,57 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.27144893211074855"/>
+                  <c:y val="4.5766768315810231E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="pt-BR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Geometry!$A$13:$A$29</c:f>
@@ -1012,6 +1240,51 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="4"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="pt-BR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Geometry!$A$13:$A$29</c:f>
@@ -10988,8 +11261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D8ECE6F-1BC1-4B28-99DF-082977825B01}">
   <dimension ref="A1:T52"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12004,8 +12277,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -12013,7 +12287,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C41090C-7CEF-4810-9952-1E4AB4D20F19}">
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="K70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
@@ -12833,6 +13107,642 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9922124A-C70C-4200-B56E-EDEBDF1F8A8C}">
+  <dimension ref="A1:Y18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" s="15">
+        <f>ATAN($G$12/(PI()*68*A1))*(180/PI())</f>
+        <v>30.333117714712536</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="P1" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q1" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="R1" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="S1" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="T1" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="U1" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="V1" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="W1" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="X1" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y1" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A2" s="11">
+        <v>0.25</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="15">
+        <f t="shared" ref="E2:E11" si="0">ATAN($G$12/(PI()*68*A2))*(180/PI())</f>
+        <v>25.084424338814244</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="O2" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="P2" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q2" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="R2" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="S2" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="T2" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="U2" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="V2" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="W2" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="X2" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y2" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A3" s="11">
+        <v>0.3</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" s="15">
+        <f t="shared" si="0"/>
+        <v>21.310042749155958</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="N3" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="O3" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="P3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q3" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="R3" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="S3" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="T3" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="U3" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="V3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="W3" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="X3" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y3" s="12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A4" s="11">
+        <v>0.35</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" s="15">
+        <f t="shared" si="0"/>
+        <v>18.487828670437434</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A5" s="11">
+        <v>0.4</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E5" s="15">
+        <f t="shared" si="0"/>
+        <v>16.307588203007903</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A6" s="11">
+        <v>0.45</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="E6" s="15">
+        <f t="shared" si="0"/>
+        <v>14.577280403880531</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A7" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E7" s="15">
+        <f t="shared" si="0"/>
+        <v>13.17303327236989</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A8" s="11">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E8" s="15">
+        <f t="shared" si="0"/>
+        <v>12.011918580323494</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="G8" s="14"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A9" s="11">
+        <v>0.6</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="E9" s="15">
+        <f t="shared" si="0"/>
+        <v>11.036572649595458</v>
+      </c>
+      <c r="F9" s="14">
+        <f>15.8*PI()/180</f>
+        <v>0.27576202181510406</v>
+      </c>
+      <c r="G9" s="14"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A10" s="11">
+        <v>0.65</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="E10" s="15">
+        <f t="shared" si="0"/>
+        <v>10.206167439276241</v>
+      </c>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A11" s="11">
+        <v>0.7</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="E11" s="15">
+        <f t="shared" si="0"/>
+        <v>9.4909123334955297</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="G11" s="14"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A12" s="11">
+        <v>0.75</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="E12" s="15">
+        <f>ATAN($G$12/(PI()*68*A12))*(180/PI())</f>
+        <v>8.8685922364362959</v>
+      </c>
+      <c r="F12" s="14">
+        <f>TAN(F9)*PI()*57*0.75</f>
+        <v>38.003942624467363</v>
+      </c>
+      <c r="G12" s="14">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A13" s="11">
+        <v>0.8</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="E13" s="15">
+        <f>ATAN($G$12/(PI()*68*A13))*(180/PI())</f>
+        <v>8.3223212859132119</v>
+      </c>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A14" s="11">
+        <v>0.85</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="E14" s="15">
+        <f t="shared" ref="E14:E18" si="1">ATAN($G$12/(PI()*68*A14))*(180/PI())</f>
+        <v>7.839045552881033</v>
+      </c>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A15" s="11">
+        <v>0.9</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="E15" s="15">
+        <f t="shared" si="1"/>
+        <v>7.4085206345962185</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A16" s="11">
+        <v>0.95</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="E16" s="15">
+        <f t="shared" si="1"/>
+        <v>7.0225982550874546</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="11">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="E17" s="15">
+        <f t="shared" si="1"/>
+        <v>6.8442618475296575</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="11">
+        <v>0.99</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="E18" s="15">
+        <f t="shared" si="1"/>
+        <v>6.7415226070051713</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D860DD4B-051B-4086-BFBF-851B739CAEA6}">
+  <dimension ref="D1:D31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D1" s="16"/>
+    </row>
+    <row r="2" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D2" s="16"/>
+    </row>
+    <row r="3" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D3" s="16"/>
+    </row>
+    <row r="4" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D4" s="16"/>
+    </row>
+    <row r="5" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D5" s="16"/>
+    </row>
+    <row r="6" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D6" s="16"/>
+    </row>
+    <row r="7" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D7" s="16"/>
+    </row>
+    <row r="8" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D8" s="16"/>
+    </row>
+    <row r="9" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D9" s="16"/>
+    </row>
+    <row r="10" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D10" s="16"/>
+    </row>
+    <row r="11" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D11" s="16"/>
+    </row>
+    <row r="12" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D12" s="16"/>
+    </row>
+    <row r="13" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D13" s="16"/>
+    </row>
+    <row r="14" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D14" s="16"/>
+    </row>
+    <row r="15" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D15" s="16"/>
+    </row>
+    <row r="16" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D16" s="16"/>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D17" s="16"/>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D18" s="16"/>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D19" s="16"/>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D20" s="16"/>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D21" s="16"/>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D22" s="16"/>
+    </row>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D23" s="16"/>
+    </row>
+    <row r="24" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D24" s="16"/>
+    </row>
+    <row r="25" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D25" s="16"/>
+    </row>
+    <row r="26" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D26" s="16"/>
+    </row>
+    <row r="27" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D27" s="16"/>
+    </row>
+    <row r="28" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D28" s="16"/>
+    </row>
+    <row r="29" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D29" s="16"/>
+    </row>
+    <row r="30" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D30" s="16"/>
+    </row>
+    <row r="31" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D31" s="16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -12844,15 +13754,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100D8FFCB9A0D31BE40A44EAC84FB9381BE" ma:contentTypeVersion="12" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="382053c858989b8f7d992e6b9e34b932">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6360b1be-1472-47f6-a243-32c73c7a856b" xmlns:ns3="6564aa30-71c4-494b-a777-08451b51a13d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cfae436508449a35691dd68c0829e949" ns2:_="" ns3:_="">
     <xsd:import namespace="6360b1be-1472-47f6-a243-32c73c7a856b"/>
@@ -13063,6 +13964,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD3452B9-8D71-4854-B596-21F7C85A760B}">
   <ds:schemaRefs>
@@ -13081,13 +13991,28 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAC98909-8B53-45EA-9C1C-81C2DCCB1776}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="6360b1be-1472-47f6-a243-32c73c7a856b"/>
+    <ds:schemaRef ds:uri="6564aa30-71c4-494b-a777-08451b51a13d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47467775-FC43-4639-A360-47D2F463F556}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAC98909-8B53-45EA-9C1C-81C2DCCB1776}"/>
 </file>
</xml_diff>